<commit_message>
Improving Performance of Code
Switching to BatuseLive3 code to improve performance
</commit_message>
<xml_diff>
--- a/BatteryCals.xlsx
+++ b/BatteryCals.xlsx
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:O264"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,7 +875,7 @@
         <v>64.67</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>11</v>
       </c>
@@ -902,7 +902,7 @@
         <v>126.59</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>12</v>
       </c>
@@ -929,7 +929,7 @@
         <v>125.71</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>13</v>
       </c>
@@ -956,7 +956,7 @@
         <v>124.08</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>13</v>
       </c>
@@ -964,7 +964,7 @@
         <v>8788</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ref="G20:G28" si="4">F20-E20</f>
+        <f t="shared" ref="G20:G26" si="4">F20-E20</f>
         <v>8788</v>
       </c>
       <c r="H20" s="1">
@@ -983,7 +983,7 @@
         <v>132.13999999999999</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>15</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>136.12</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>16</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>135.41</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>17</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>142.85</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>18</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>125.72</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>19</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>140.29</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D26">
         <v>20</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>131.35</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D27">
         <v>21</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>134.43</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D28">
         <v>22</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>139.97</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I29" s="1">
         <f>SUM(I6:I28)</f>
         <v>28447.66066128069</v>
@@ -1208,97 +1208,119 @@
         <v>126.24</v>
       </c>
     </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.2">
       <c r="O30">
         <v>141.04</v>
       </c>
     </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
       <c r="O31">
         <v>144.19999999999999</v>
       </c>
     </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <f>0.8</f>
+        <v>0.8</v>
+      </c>
       <c r="O32">
         <v>147.25</v>
       </c>
     </row>
-    <row r="33" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <f>C32*E32</f>
+        <v>160</v>
+      </c>
       <c r="O33">
         <v>140.44999999999999</v>
       </c>
     </row>
-    <row r="34" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <f>(C32-E33)/D32</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="O34">
         <v>125.38</v>
       </c>
     </row>
-    <row r="35" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f>5000/190</f>
+        <v>26.315789473684209</v>
+      </c>
       <c r="O35">
         <v>135.9</v>
       </c>
     </row>
-    <row r="36" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O36">
         <v>134.34</v>
       </c>
     </row>
-    <row r="37" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O37">
         <v>139.66999999999999</v>
       </c>
     </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O38">
         <v>139.47</v>
       </c>
     </row>
-    <row r="39" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O39">
         <v>115.39</v>
       </c>
     </row>
-    <row r="40" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O40">
         <v>141.13</v>
       </c>
     </row>
-    <row r="41" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O41">
         <v>143.85</v>
       </c>
     </row>
-    <row r="42" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O42">
         <v>141.85</v>
       </c>
     </row>
-    <row r="43" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O43">
         <v>145.22999999999999</v>
       </c>
     </row>
-    <row r="44" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O44">
         <v>129.4</v>
       </c>
     </row>
-    <row r="45" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O45">
         <v>140.79</v>
       </c>
     </row>
-    <row r="46" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O46">
         <v>152.63999999999999</v>
       </c>
     </row>
-    <row r="47" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O47">
         <v>144.27000000000001</v>
       </c>
     </row>
-    <row r="48" spans="15:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O48">
         <v>148.37</v>
       </c>

</xml_diff>